<commit_message>
change port and add xr
</commit_message>
<xml_diff>
--- a/static/data/show_command.xlsx
+++ b/static/data/show_command.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="229">
   <si>
     <t xml:space="preserve">cisco_ios</t>
   </si>
@@ -598,6 +598,9 @@
     <t xml:space="preserve">show msglog</t>
   </si>
   <si>
+    <t xml:space="preserve">cisco_xr</t>
+  </si>
+  <si>
     <t xml:space="preserve">riverbed</t>
   </si>
   <si>
@@ -640,9 +643,6 @@
     <t xml:space="preserve">show hardware spec</t>
   </si>
   <si>
-    <t xml:space="preserve">show hardware error-log</t>
-  </si>
-  <si>
     <t xml:space="preserve">show stats fan</t>
   </si>
   <si>
@@ -650,9 +650,6 @@
   </si>
   <si>
     <t xml:space="preserve">show stats cpu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">show in-path neighbour</t>
   </si>
   <si>
     <t xml:space="preserve">show report all</t>
@@ -810,10 +807,10 @@
   <dimension ref="A1:DD47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.85"/>
@@ -853,7 +850,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="22.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="26.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="31.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="37.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="46" style="0" width="21.71"/>
@@ -889,7 +886,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="81" min="81" style="0" width="28.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="0" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="0" width="26.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="83" style="0" width="20.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="85" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="86" min="86" style="0" width="26.42"/>
@@ -898,7 +895,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="89" style="0" width="18.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="90" min="90" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="91" min="91" style="0" width="32.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="92" style="0" width="38.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="92" style="0" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="95" style="0" width="10.57"/>
@@ -1985,133 +1982,452 @@
         <v>192</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP6" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ6" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS6" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT6" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU6" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AX6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AZ6" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB6" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="BC6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="BD6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="BE6" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="BF6" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="BG6" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="BH6" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="BJ6" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="BK6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="BL6" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="BM6" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="BN6" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="BO6" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="BP6" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="BQ6" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="BR6" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="BS6" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="BT6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="BU6" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="BV6" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="BW6" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="BX6" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="BY6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="BZ6" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="CA6" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="CB6" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="CC6" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="CD6" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="CE6" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="CF6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="CG6" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="CH6" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="CI6" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="CJ6" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="CK6" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="CL6" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="CM6" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="CN6" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="CO6" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="CP6" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="CQ6" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="CR6" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="CS6" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="CT6" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="CU6" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="CV6" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="CW6" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="CX6" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="CY6" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="CZ6" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="DA6" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="DB6" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="DC6" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="DD6" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="D6" s="0" t="s">
+      <c r="C7" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="G6" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="H7" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="I7" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="L6" s="0" t="s">
+      <c r="K7" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="L7" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="N6" s="0" t="s">
+      <c r="M7" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="O6" s="0" t="s">
+      <c r="N7" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="P6" s="0" t="s">
+      <c r="O7" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="P7" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="R6" s="0" t="s">
+      <c r="Q7" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="S6" s="0" t="s">
+      <c r="R7" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="T6" s="0" t="s">
+      <c r="S7" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="U6" s="0" t="s">
+      <c r="T7" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="V6" s="0" t="s">
+      <c r="U7" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="W6" s="0" t="s">
+      <c r="V7" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="X6" s="0" t="s">
+      <c r="W7" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="Y6" s="0" t="s">
+      <c r="X7" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="Z6" s="0" t="s">
+      <c r="Y7" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="AA6" s="0" t="s">
+      <c r="Z7" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="AB6" s="0" t="s">
+      <c r="AA7" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="AC6" s="0" t="s">
+      <c r="AB7" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="AD6" s="0" t="s">
+      <c r="AC7" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="AE6" s="0" t="s">
+      <c r="AD7" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="AF6" s="0" t="s">
+      <c r="AE7" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="AG6" s="0" t="s">
+      <c r="AF7" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="AH6" s="0" t="s">
+      <c r="AG7" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="AI6" s="0" t="s">
+      <c r="AH7" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="AJ6" s="0" t="s">
+      <c r="AI7" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="AK6" s="0" t="s">
+      <c r="AJ7" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="AL6" s="0" t="s">
+      <c r="AK7" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="AM6" s="0" t="s">
+      <c r="AL7" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM7" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="AN6" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="AO6" s="0" t="s">
+      <c r="AN7" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="AP6" s="0" t="s">
+      <c r="AO7" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="AQ6" s="0" t="s">
-        <v>229</v>
-      </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
adding sg series for felix
</commit_message>
<xml_diff>
--- a/static/data/show_command.xlsx
+++ b/static/data/show_command.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="239">
   <si>
     <t xml:space="preserve">cisco_ios_telnet</t>
   </si>
@@ -328,6 +328,30 @@
     <t xml:space="preserve">show bgp filter-list</t>
   </si>
   <si>
+    <t xml:space="preserve">show cpu utilization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show memory statistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show dir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show vlan default-vlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show ip access-lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show etherchannel summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show power inline consumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show mac address-table</t>
+  </si>
+  <si>
     <t xml:space="preserve">clear log</t>
   </si>
   <si>
@@ -425,9 +449,6 @@
   </si>
   <si>
     <t xml:space="preserve">show int transceiver details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">show mac address-table</t>
   </si>
   <si>
     <t xml:space="preserve">show flogi database</t>
@@ -791,8 +812,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -813,451 +838,487 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:DF8"/>
+  <dimension ref="A1:DN8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AV1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AY9" activeCellId="0" sqref="AY9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="31.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="36.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="25.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="17.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="31.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="24.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="37.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="46" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="15.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="52" style="0" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="27.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="56" style="0" width="30.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="37.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="27.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="0" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="0" width="30.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="0" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="0" width="23.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="0" width="30.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="0" width="29.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="31.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="0" width="25.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="77" style="0" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="0" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="0" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="81" min="81" style="0" width="28.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="0" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="83" style="0" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="85" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="86" min="86" style="0" width="26.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="87" min="87" style="0" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="88" min="88" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="89" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="90" min="90" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="91" min="91" style="0" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="92" style="0" width="38.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="0" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="95" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="96" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="97" style="0" width="41.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="0" width="41.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="99" style="0" width="28.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="101" style="0" width="26.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="102" style="0" width="6.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="103" min="103" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="104" min="104" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="105" min="105" style="0" width="49.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="106" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="107" min="107" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="108" min="108" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="29.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="32.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="29.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="26.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="34.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="24.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="0" width="38.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="27.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="0" width="38.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="40.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="25.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="24.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="20.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="25.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="29.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="21.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="27.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="23.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="29.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="35.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="22.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="21.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="28.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="0" width="28.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="21.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="23.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="18.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="0" width="23.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="0" width="18.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="0" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="0" width="28.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="30.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="76" style="0" width="27.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="0" width="22.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="0" width="28.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="81" min="81" style="0" width="28.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="0" width="24.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="84" style="0" width="15.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="85" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="86" min="86" style="0" width="25.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="87" min="87" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="88" min="88" style="0" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="89" style="0" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="90" min="90" style="0" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="91" style="0" width="21.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="0" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="95" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="96" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="97" style="0" width="38.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="0" width="38.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="99" style="0" width="27.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="0" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="101" style="0" width="25.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="102" style="0" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="103" min="103" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="104" min="104" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="105" min="105" style="0" width="46.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="106" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="107" min="107" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="108" min="108" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="109" min="109" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="110" min="110" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="111" min="111" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="112" min="112" style="0" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="113" min="113" style="0" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="114" min="114" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="115" min="115" style="0" width="25.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="116" min="116" style="0" width="28.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="117" min="117" style="0" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="118" min="118" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="119" min="119" style="0" width="12.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AI1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="0" t="s">
+      <c r="AK1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="0" t="s">
+      <c r="AL1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="0" t="s">
+      <c r="AM1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="0" t="s">
+      <c r="AN1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="0" t="s">
+      <c r="AO1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="0" t="s">
+      <c r="AP1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" s="0" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" s="0" t="s">
+      <c r="AR1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" s="0" t="s">
+      <c r="AS1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AT1" s="0" t="s">
+      <c r="AT1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AU1" s="0" t="s">
+      <c r="AU1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" s="0" t="s">
+      <c r="AV1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AW1" s="0" t="s">
+      <c r="AW1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AX1" s="0" t="s">
+      <c r="AX1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AY1" s="0" t="s">
+      <c r="AY1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" s="0" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" s="0" t="s">
+      <c r="BA1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" s="0" t="s">
+      <c r="BB1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BC1" s="0" t="s">
+      <c r="BC1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BD1" s="0" t="s">
+      <c r="BD1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BE1" s="0" t="s">
+      <c r="BE1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BF1" s="0" t="s">
+      <c r="BF1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BG1" s="0" t="s">
+      <c r="BG1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BH1" s="0" t="s">
+      <c r="BH1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BI1" s="0" t="s">
+      <c r="BI1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BJ1" s="0" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BK1" s="0" t="s">
+      <c r="BK1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BL1" s="0" t="s">
+      <c r="BL1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BM1" s="0" t="s">
+      <c r="BM1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BN1" s="0" t="s">
+      <c r="BN1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BO1" s="0" t="s">
+      <c r="BO1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BP1" s="0" t="s">
+      <c r="BP1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BQ1" s="0" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BR1" s="0" t="s">
+      <c r="BR1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BS1" s="0" t="s">
+      <c r="BS1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BT1" s="0" t="s">
+      <c r="BT1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BU1" s="0" t="s">
+      <c r="BU1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BV1" s="0" t="s">
+      <c r="BV1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BW1" s="0" t="s">
+      <c r="BW1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BX1" s="0" t="s">
+      <c r="BX1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BY1" s="0" t="s">
+      <c r="BY1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="BZ1" s="0" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="CA1" s="0" t="s">
+      <c r="CA1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="CB1" s="0" t="s">
+      <c r="CB1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="CC1" s="0" t="s">
+      <c r="CC1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="CD1" s="0" t="s">
+      <c r="CD1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="CE1" s="0" t="s">
+      <c r="CE1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="CF1" s="0" t="s">
+      <c r="CF1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="CG1" s="0" t="s">
+      <c r="CG1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="CH1" s="0" t="s">
+      <c r="CH1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="CI1" s="0" t="s">
+      <c r="CI1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CJ1" s="0" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CK1" s="0" t="s">
+      <c r="CK1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CL1" s="0" t="s">
+      <c r="CL1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CM1" s="0" t="s">
+      <c r="CM1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CN1" s="0" t="s">
+      <c r="CN1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CO1" s="0" t="s">
+      <c r="CO1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CP1" s="0" t="s">
+      <c r="CP1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CQ1" s="0" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CR1" s="0" t="s">
+      <c r="CR1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="CS1" s="0" t="s">
+      <c r="CS1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CT1" s="0" t="s">
+      <c r="CT1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CU1" s="0" t="s">
+      <c r="CU1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CV1" s="0" t="s">
+      <c r="CV1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="CW1" s="0" t="s">
+      <c r="CW1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="CX1" s="0" t="s">
+      <c r="CX1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="CY1" s="0" t="s">
+      <c r="CY1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="CZ1" s="0" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="DA1" s="0" t="s">
+      <c r="DA1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="DB1" s="0" t="s">
+      <c r="DB1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="DC1" s="0" t="s">
+      <c r="DC1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="DD1" s="0" t="s">
+      <c r="DD1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="DE1" s="0" t="s">
+      <c r="DE1" s="1" t="s">
         <v>102</v>
       </c>
       <c r="DF1" s="0" t="s">
         <v>103</v>
+      </c>
+      <c r="DG1" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="DH1" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="DI1" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="DJ1" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="DK1" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="DL1" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="DM1" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="DN1" s="0" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>1</v>
@@ -1585,11 +1646,35 @@
       </c>
       <c r="DF2" s="0" t="s">
         <v>103</v>
+      </c>
+      <c r="DG2" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="DH2" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="DI2" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="DJ2" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="DK2" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="DL2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="DM2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="DN2" s="0" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>1</v>
@@ -1598,7 +1683,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>4</v>
@@ -1607,7 +1692,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>7</v>
@@ -1616,7 +1701,7 @@
         <v>8</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K3" s="0" t="s">
         <v>10</v>
@@ -1913,33 +1998,33 @@
         <v>101</v>
       </c>
       <c r="DE3" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="DF3" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>7</v>
@@ -1948,7 +2033,7 @@
         <v>8</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K4" s="0" t="s">
         <v>10</v>
@@ -1957,51 +2042,51 @@
         <v>84</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="Q4" s="0" t="s">
         <v>97</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="V4" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>4</v>
@@ -2010,7 +2095,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>7</v>
@@ -2019,34 +2104,34 @@
         <v>8</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>10</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="T5" s="0" t="s">
         <v>11</v>
@@ -2055,10 +2140,10 @@
         <v>72</v>
       </c>
       <c r="V5" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="X5" s="0" t="s">
         <v>32</v>
@@ -2067,13 +2152,13 @@
         <v>64</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="AA5" s="0" t="s">
         <v>65</v>
       </c>
       <c r="AB5" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="AC5" s="0" t="s">
         <v>38</v>
@@ -2082,127 +2167,127 @@
         <v>84</v>
       </c>
       <c r="AE5" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="AF5" s="0" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="AG5" s="0" t="s">
         <v>33</v>
       </c>
       <c r="AH5" s="0" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="AI5" s="0" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="AJ5" s="0" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="AK5" s="0" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="AL5" s="0" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="AM5" s="0" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="AN5" s="0" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="AO5" s="0" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="AP5" s="0" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="AQ5" s="0" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="AR5" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="AS5" s="0" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="AT5" s="0" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="AU5" s="0" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="AV5" s="0" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="AW5" s="0" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="AX5" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="AY5" s="0" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="AZ5" s="0" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="BA5" s="0" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="BB5" s="0" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="BC5" s="0" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="BD5" s="0" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="BE5" s="0" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="BF5" s="0" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="BG5" s="0" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="BH5" s="0" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="BI5" s="0" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="BJ5" s="0" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="BK5" s="0" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="BL5" s="0" t="s">
         <v>20</v>
       </c>
       <c r="BM5" s="0" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="BN5" s="0" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="BO5" s="0" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="BP5" s="0" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="BQ5" s="0" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="BR5" s="0" t="s">
         <v>63</v>
       </c>
       <c r="BS5" s="0" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="BT5" s="0" t="s">
         <v>75</v>
@@ -2217,37 +2302,37 @@
         <v>52</v>
       </c>
       <c r="BX5" s="0" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="BY5" s="0" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="BZ5" s="0" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="CA5" s="0" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="CB5" s="0" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="CC5" s="0" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="CD5" s="0" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="CE5" s="0" t="s">
         <v>29</v>
       </c>
       <c r="CF5" s="0" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="CG5" s="0" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="CH5" s="0" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="CI5" s="0" t="s">
         <v>39</v>
@@ -2268,39 +2353,39 @@
         <v>44</v>
       </c>
       <c r="CO5" s="0" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="CP5" s="0" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="CQ5" s="0" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="CR5" s="0" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="CS5" s="0" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="CT5" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="CU5" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>4</v>
@@ -2309,57 +2394,57 @@
         <v>5</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S6" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="N6" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="P6" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="R6" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="S6" s="0" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>4</v>
@@ -2368,7 +2453,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>7</v>
@@ -2377,7 +2462,7 @@
         <v>8</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>10</v>
@@ -2674,21 +2759,21 @@
         <v>101</v>
       </c>
       <c r="DE7" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="DF7" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>6</v>
@@ -2697,112 +2782,112 @@
         <v>11</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="J8" s="0" t="s">
         <v>24</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="V8" s="0" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="Y8" s="0" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="AA8" s="0" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="AB8" s="0" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="AC8" s="0" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="AD8" s="0" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="AE8" s="0" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="AF8" s="0" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="AG8" s="0" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="AH8" s="0" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="AI8" s="0" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="AJ8" s="0" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="AK8" s="0" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="AL8" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="AM8" s="0" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="AN8" s="0" t="s">
         <v>2</v>
       </c>
       <c r="AO8" s="0" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing error command cucm
</commit_message>
<xml_diff>
--- a/static/data/show_command.xlsx
+++ b/static/data/show_command.xlsx
@@ -739,7 +739,7 @@
     <t xml:space="preserve">show protocol ssl expiring-certs</t>
   </si>
   <si>
-    <t xml:space="preserve">cucm</t>
+    <t xml:space="preserve">ucm</t>
   </si>
   <si>
     <t xml:space="preserve">show network cluster</t>
@@ -880,10 +880,10 @@
   <dimension ref="A1:DN9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.62"/>
@@ -900,10 +900,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="29.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="32.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="32.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="29.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="26.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="26.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="34.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="24.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="20.05"/>
@@ -927,11 +927,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="20.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="21.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="29.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="35.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="14.62"/>
@@ -939,7 +939,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="21.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="34.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="21.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="25.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="28.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="0" width="28.38"/>
@@ -947,7 +947,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="21.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="23.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="18.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="21.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="0" width="23.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="0" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="0" width="26.59"/>
@@ -973,7 +973,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="0" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="95" style="0" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="96" style="0" width="24.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="96" style="0" width="24.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="97" style="0" width="38.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="0" width="38.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="99" style="0" width="27.41"/>

</xml_diff>

<commit_message>
adding new command to cucm
</commit_message>
<xml_diff>
--- a/static/data/show_command.xlsx
+++ b/static/data/show_command.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="253">
   <si>
     <t xml:space="preserve">cisco_ios_telnet</t>
   </si>
@@ -775,7 +775,10 @@
     <t xml:space="preserve">show risdb query phone</t>
   </si>
   <si>
-    <t xml:space="preserve">file tail activelog /cm/log/amc/AlertLog/AlertLog_11_03_2020_09_36.csv 30</t>
+    <t xml:space="preserve">show risdb query phoneextn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run sql select name,tkmodel from TypeProduct</t>
   </si>
 </sst>
 </file>
@@ -879,11 +882,11 @@
   </sheetPr>
   <dimension ref="A1:DN9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M9" activeCellId="0" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.62"/>
@@ -2972,6 +2975,9 @@
       <c r="N9" s="0" t="s">
         <v>251</v>
       </c>
+      <c r="O9" s="0" t="s">
+        <v>252</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update command and logic cucm
</commit_message>
<xml_diff>
--- a/static/data/show_command.xlsx
+++ b/static/data/show_command.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="255">
   <si>
     <t xml:space="preserve">cisco_ios_telnet</t>
   </si>
@@ -779,6 +779,12 @@
   </si>
   <si>
     <t xml:space="preserve">run sql select name,tkmodel from TypeProduct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show cert list own</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file list activelog /cm/log/amc/AlertLog reverse date</t>
   </si>
 </sst>
 </file>
@@ -882,11 +888,11 @@
   </sheetPr>
   <dimension ref="A1:DN9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M9" activeCellId="0" sqref="M9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q10" activeCellId="0" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.62"/>
@@ -2978,6 +2984,12 @@
       <c r="O9" s="0" t="s">
         <v>252</v>
       </c>
+      <c r="P9" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>254</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add utils diagnose test to command
</commit_message>
<xml_diff>
--- a/static/data/show_command.xlsx
+++ b/static/data/show_command.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATION\virtualenv\compnet\netoprmgr_dm\Lib\site-packages\netoprmgr_dm\static\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luthfi.anandra.COMPNET\virtual_environments\netoprmgr_dm\venv_netoprmgr_dm\Lib\site-packages\netoprmgr_dm\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28CC427-0C6F-4E1A-B48D-A6DECC931683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69615BF0-1888-4598-8AE4-B4D370D6DA7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="263">
   <si>
     <t>cisco_ios_telnet</t>
   </si>
@@ -811,6 +811,9 @@
   </si>
   <si>
     <t>run cuc dbquery unitymbxdb1 select alias as UserID, count (*) as messages, sum(case when deleted='0' then 1 else 0 end) as Inboxmessages, sum(case when deleted='1' then 1 else 0 end) as Deletedmessages from vw_message, unitydirdb: vw_mailbox, unitydirdb:vw_user where mailboxobjectid in (select mailboxid from vw_mailbox where unitydirdb:vw_user.objectid = unitydirdb:vw_mailbox.userobjectid) group by alias order by messages desc</t>
+  </si>
+  <si>
+    <t>utils diagnose test</t>
   </si>
 </sst>
 </file>
@@ -1165,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DN9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3288,6 +3291,9 @@
       <c r="X9" t="s">
         <v>254</v>
       </c>
+      <c r="Y9" t="s">
+        <v>262</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
remove f5 folder, add command f5 di xlsx
</commit_message>
<xml_diff>
--- a/static/data/show_command.xlsx
+++ b/static/data/show_command.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="313">
   <si>
     <t xml:space="preserve">cisco_ios_telnet</t>
   </si>
@@ -911,6 +911,54 @@
   </si>
   <si>
     <t xml:space="preserve">tmsh list sys global-settings hostname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh show sys version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uptime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh show sys hardware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh show sys performance system historical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh show sys performance throughput historical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh show sys performance connections historical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh -q -c "cd /;show ltm virtual recursive" | grep -iE "(ltm::virtual|availability|state)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh -q -c "cd /;show ltm pool recursive" | grep -iE "(ltm::pool|availability|state)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh -q -c "cd /;show ltm node recursive" | grep -iE "(ltm::node|availability|state)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh show cm device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh show cm sync-status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh show cm traffic-group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh -q -c "cd /; list sys file ssl-cert recursive"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh show sys license</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmsh show sys provision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cat /var/log/ltm</t>
   </si>
 </sst>
 </file>
@@ -986,7 +1034,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -996,6 +1044,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1018,8 +1070,8 @@
   </sheetPr>
   <dimension ref="A1:DN15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S13" activeCellId="0" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2267,7 +2319,7 @@
       <c r="D5" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="3" t="s">
         <v>130</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -3306,27 +3358,63 @@
       <c r="B13" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="G13" s="0"/>
-      <c r="H13" s="0"/>
-      <c r="I13" s="0"/>
-      <c r="J13" s="0"/>
-      <c r="K13" s="0"/>
-      <c r="L13" s="0"/>
-      <c r="M13" s="0"/>
-      <c r="N13" s="0"/>
-      <c r="O13" s="0"/>
-      <c r="P13" s="0"/>
-      <c r="Q13" s="0"/>
-      <c r="R13" s="0"/>
+      <c r="C13" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O14" s="0"/>
-      <c r="P14" s="0"/>
-      <c r="Q14" s="0"/>
-      <c r="R14" s="0"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
+      <c r="B15" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>